<commit_message>
2017-02-13 snapshot - chunk 36
</commit_message>
<xml_diff>
--- a/www.eia.gov/outlooks/steo/xls/Fig1.xlsx
+++ b/www.eia.gov/outlooks/steo/xls/Fig1.xlsx
@@ -32,7 +32,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
-    <t>Short-Term Energy Outlook, January 2017</t>
+    <t>Short-Term Energy Outlook, February 2017</t>
   </si>
   <si>
     <t>Change the confidence interval by entering a</t>
@@ -80,10 +80,10 @@
     <t>Upper</t>
   </si>
   <si>
-    <t>Source: Short-Term Energy Outlook, January 2017.</t>
+    <t>Source: Short-Term Energy Outlook, February 2017.</t>
   </si>
   <si>
-    <t>Note: Confidence interval derived from options market information for the 5 trading days ending Jan 5, 2017. Intervals not calculated for months with sparse trading in near-the-money options contracts.</t>
+    <t>Note: Confidence interval derived from options market information for the 5 trading days ending Feb 2, 2017. Intervals not calculated for months with sparse trading in near-the-money options contracts.</t>
   </si>
   <si>
     <t>Where:</t>
@@ -522,13 +522,13 @@
                   <c:v>49.774999999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45.71</c:v>
+                  <c:v>45.661000000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>51.97</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>#N/A</c:v>
+                  <c:v>52.49</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>#N/A</c:v>
@@ -777,79 +777,79 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>51.97</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>52</c:v>
+                  <c:v>52.49</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>52</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>52</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>52</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>52</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>52</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>53</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>53</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>53</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>53</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>53</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>53</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>53</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>53</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>53</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>54</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>55</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>55</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>55</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>56</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>56</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>57</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>57</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>58</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1038,70 +1038,70 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>54.314</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>55.116</c:v>
+                  <c:v>53.814000000000007</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>55.777999999999999</c:v>
+                  <c:v>54.326000000000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>56.265999999999998</c:v>
+                  <c:v>54.757999999999996</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>56.573999999999998</c:v>
+                  <c:v>55.064</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>56.741999999999997</c:v>
+                  <c:v>55.25</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>56.844000000000008</c:v>
+                  <c:v>55.379999999999995</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>56.894000000000005</c:v>
+                  <c:v>55.470000000000006</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>56.922000000000004</c:v>
+                  <c:v>55.548000000000002</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>56.944000000000003</c:v>
+                  <c:v>55.616</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>56.884</c:v>
+                  <c:v>55.660000000000004</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>56.823999999999998</c:v>
+                  <c:v>55.694000000000003</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>56.754000000000005</c:v>
+                  <c:v>55.731999999999992</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>56.679999999999993</c:v>
+                  <c:v>55.738</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>56.60799999999999</c:v>
+                  <c:v>55.736000000000004</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>56.564</c:v>
+                  <c:v>55.725999999999999</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>56.486000000000004</c:v>
+                  <c:v>55.679999999999993</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>56.427999999999997</c:v>
+                  <c:v>55.646000000000001</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>56.402000000000001</c:v>
+                  <c:v>55.620000000000005</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>56.386000000000003</c:v>
+                  <c:v>55.608000000000004</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>56.379999999999995</c:v>
+                  <c:v>55.606000000000009</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>56.383999999999993</c:v>
+                  <c:v>55.622</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1308,70 +1308,70 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>44.992506655000135</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43.091772909633576</c:v>
+                  <c:v>44.542492128643843</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>41.598697955469788</c:v>
+                  <c:v>42.334181145273284</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>40.105096853756812</c:v>
+                  <c:v>40.298775355191346</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>38.837387675060832</c:v>
+                  <c:v>38.656357360969729</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>37.920401356633704</c:v>
+                  <c:v>37.588664956469671</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>36.860305349127543</c:v>
+                  <c:v>36.342571643368707</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>36.04716912997808</c:v>
+                  <c:v>35.503151838856461</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>35.326408825942011</c:v>
+                  <c:v>34.711726970930016</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>34.818118559944736</c:v>
+                  <c:v>34.068320116932881</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>#N/A</c:v>
+                  <c:v>33.381601430531042</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>#N/A</c:v>
+                  <c:v>32.906422271354188</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>#N/A</c:v>
+                  <c:v>32.42676407210547</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>#N/A</c:v>
+                  <c:v>32.033729548552806</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>#N/A</c:v>
+                  <c:v>31.622050174373111</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>32.021640238413859</c:v>
+                  <c:v>31.421745124934933</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>#N/A</c:v>
+                  <c:v>30.895951939699067</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>#N/A</c:v>
+                  <c:v>30.59698227934512</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>#N/A</c:v>
+                  <c:v>30.270109390498018</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>#N/A</c:v>
+                  <c:v>30.011037641066501</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>#N/A</c:v>
+                  <c:v>29.759663551158464</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>30.097734612969429</c:v>
+                  <c:v>29.731159362954337</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1578,70 +1578,70 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>65.566709110486016</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>70.495439172818919</c:v>
+                  <c:v>65.015369765036354</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>74.790448665735511</c:v>
+                  <c:v>69.714689080020676</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>78.939162459682237</c:v>
+                  <c:v>74.405203075575258</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>82.410730164924416</c:v>
+                  <c:v>78.435846080556274</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>84.905603548860142</c:v>
+                  <c:v>81.209654653472882</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>87.661789705615718</c:v>
+                  <c:v>84.38985633972365</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>89.796988615898243</c:v>
+                  <c:v>86.666133586271116</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>91.719316842096248</c:v>
+                  <c:v>88.891581412358917</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>93.130222714858448</c:v>
+                  <c:v>90.792250553693293</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>#N/A</c:v>
+                  <c:v>92.806679944555199</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>#N/A</c:v>
+                  <c:v>94.261892417888561</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>#N/A</c:v>
+                  <c:v>95.786795657230783</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>#N/A</c:v>
+                  <c:v>96.982920433638768</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>#N/A</c:v>
+                  <c:v>98.238465844872607</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>99.916371309481718</c:v>
+                  <c:v>98.82923636649636</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>#N/A</c:v>
+                  <c:v>100.3452622547741</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>#N/A</c:v>
+                  <c:v>101.20204952663963</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>#N/A</c:v>
+                  <c:v>102.19931352382547</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>#N/A</c:v>
+                  <c:v>103.03707925675414</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>#N/A</c:v>
+                  <c:v>103.8999392813914</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>105.6277323486688</c:v>
+                  <c:v>104.05940939709703</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1657,11 +1657,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="414554768"/>
-        <c:axId val="414555328"/>
+        <c:axId val="576372000"/>
+        <c:axId val="576372560"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="414554768"/>
+        <c:axId val="576372000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1678,7 +1678,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="414555328"/>
+        <c:crossAx val="576372560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -1689,7 +1689,7 @@
         <c:minorTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="414555328"/>
+        <c:axId val="576372560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="140"/>
@@ -1717,7 +1717,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="414554768"/>
+        <c:crossAx val="576372000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="20"/>
@@ -1731,7 +1731,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.10470831389978692"/>
           <c:y val="0.12078059589285008"/>
-          <c:w val="0.6499924094853996"/>
+          <c:w val="0.62908648614045182"/>
           <c:h val="0.22246471159608991"/>
         </c:manualLayout>
       </c:layout>
@@ -2002,7 +2002,7 @@
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:pPr algn="l"/>
-            <a:t>Source: Short-Term Energy Outlook, January 2017.</a:t>
+            <a:t>Source: Short-Term Energy Outlook, February 2017.</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="900">
             <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
@@ -2047,7 +2047,7 @@
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>Note: Confidence interval derived from options market information for the 5 trading days ending Jan 5, 2017. Intervals not calculated for months with sparse trading in near-the-money options contracts.</a:t>
+            <a:t>Note: Confidence interval derived from options market information for the 5 trading days ending Feb 2, 2017. Intervals not calculated for months with sparse trading in near-the-money options contracts.</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="900">
             <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
@@ -2310,7 +2310,7 @@
             <v>42675</v>
           </cell>
           <cell r="C39">
-            <v>45.71</v>
+            <v>45.661000000000001</v>
           </cell>
           <cell r="D39" t="e">
             <v>#N/A</v>
@@ -2332,8 +2332,8 @@
           <cell r="C40">
             <v>51.97</v>
           </cell>
-          <cell r="D40">
-            <v>51.97</v>
+          <cell r="D40" t="e">
+            <v>#N/A</v>
           </cell>
           <cell r="E40" t="e">
             <v>#N/A</v>
@@ -2349,11 +2349,11 @@
           <cell r="B41">
             <v>42736</v>
           </cell>
-          <cell r="C41" t="e">
-            <v>#N/A</v>
+          <cell r="C41">
+            <v>52.49</v>
           </cell>
           <cell r="D41">
-            <v>52</v>
+            <v>52.49</v>
           </cell>
           <cell r="E41" t="e">
             <v>#N/A</v>
@@ -2373,7 +2373,7 @@
             <v>#N/A</v>
           </cell>
           <cell r="D42">
-            <v>52</v>
+            <v>53</v>
           </cell>
           <cell r="E42" t="e">
             <v>#N/A</v>
@@ -2393,16 +2393,16 @@
             <v>#N/A</v>
           </cell>
           <cell r="D43">
-            <v>52</v>
-          </cell>
-          <cell r="E43">
-            <v>54.314</v>
-          </cell>
-          <cell r="H43">
-            <v>44.992506655000135</v>
-          </cell>
-          <cell r="I43">
-            <v>65.566709110486016</v>
+            <v>53</v>
+          </cell>
+          <cell r="E43" t="e">
+            <v>#N/A</v>
+          </cell>
+          <cell r="H43" t="e">
+            <v>#N/A</v>
+          </cell>
+          <cell r="I43" t="e">
+            <v>#N/A</v>
           </cell>
         </row>
         <row r="44">
@@ -2413,16 +2413,16 @@
             <v>#N/A</v>
           </cell>
           <cell r="D44">
-            <v>52</v>
+            <v>53</v>
           </cell>
           <cell r="E44">
-            <v>55.116</v>
+            <v>53.814000000000007</v>
           </cell>
           <cell r="H44">
-            <v>43.091772909633576</v>
+            <v>44.542492128643843</v>
           </cell>
           <cell r="I44">
-            <v>70.495439172818919</v>
+            <v>65.015369765036354</v>
           </cell>
         </row>
         <row r="45">
@@ -2433,16 +2433,16 @@
             <v>#N/A</v>
           </cell>
           <cell r="D45">
-            <v>52</v>
+            <v>53</v>
           </cell>
           <cell r="E45">
-            <v>55.777999999999999</v>
+            <v>54.326000000000001</v>
           </cell>
           <cell r="H45">
-            <v>41.598697955469788</v>
+            <v>42.334181145273284</v>
           </cell>
           <cell r="I45">
-            <v>74.790448665735511</v>
+            <v>69.714689080020676</v>
           </cell>
         </row>
         <row r="46">
@@ -2453,16 +2453,16 @@
             <v>#N/A</v>
           </cell>
           <cell r="D46">
-            <v>52</v>
+            <v>53</v>
           </cell>
           <cell r="E46">
-            <v>56.265999999999998</v>
+            <v>54.757999999999996</v>
           </cell>
           <cell r="H46">
-            <v>40.105096853756812</v>
+            <v>40.298775355191346</v>
           </cell>
           <cell r="I46">
-            <v>78.939162459682237</v>
+            <v>74.405203075575258</v>
           </cell>
         </row>
         <row r="47">
@@ -2473,16 +2473,16 @@
             <v>#N/A</v>
           </cell>
           <cell r="D47">
-            <v>53</v>
+            <v>54</v>
           </cell>
           <cell r="E47">
-            <v>56.573999999999998</v>
+            <v>55.064</v>
           </cell>
           <cell r="H47">
-            <v>38.837387675060832</v>
+            <v>38.656357360969729</v>
           </cell>
           <cell r="I47">
-            <v>82.410730164924416</v>
+            <v>78.435846080556274</v>
           </cell>
         </row>
         <row r="48">
@@ -2493,16 +2493,16 @@
             <v>#N/A</v>
           </cell>
           <cell r="D48">
-            <v>53</v>
+            <v>54</v>
           </cell>
           <cell r="E48">
-            <v>56.741999999999997</v>
+            <v>55.25</v>
           </cell>
           <cell r="H48">
-            <v>37.920401356633704</v>
+            <v>37.588664956469671</v>
           </cell>
           <cell r="I48">
-            <v>84.905603548860142</v>
+            <v>81.209654653472882</v>
           </cell>
         </row>
         <row r="49">
@@ -2513,16 +2513,16 @@
             <v>#N/A</v>
           </cell>
           <cell r="D49">
-            <v>53</v>
+            <v>54</v>
           </cell>
           <cell r="E49">
-            <v>56.844000000000008</v>
+            <v>55.379999999999995</v>
           </cell>
           <cell r="H49">
-            <v>36.860305349127543</v>
+            <v>36.342571643368707</v>
           </cell>
           <cell r="I49">
-            <v>87.661789705615718</v>
+            <v>84.38985633972365</v>
           </cell>
         </row>
         <row r="50">
@@ -2533,16 +2533,16 @@
             <v>#N/A</v>
           </cell>
           <cell r="D50">
-            <v>53</v>
+            <v>54</v>
           </cell>
           <cell r="E50">
-            <v>56.894000000000005</v>
+            <v>55.470000000000006</v>
           </cell>
           <cell r="H50">
-            <v>36.04716912997808</v>
+            <v>35.503151838856461</v>
           </cell>
           <cell r="I50">
-            <v>89.796988615898243</v>
+            <v>86.666133586271116</v>
           </cell>
         </row>
         <row r="51">
@@ -2553,16 +2553,16 @@
             <v>#N/A</v>
           </cell>
           <cell r="D51">
-            <v>53</v>
+            <v>54</v>
           </cell>
           <cell r="E51">
-            <v>56.922000000000004</v>
+            <v>55.548000000000002</v>
           </cell>
           <cell r="H51">
-            <v>35.326408825942011</v>
+            <v>34.711726970930016</v>
           </cell>
           <cell r="I51">
-            <v>91.719316842096248</v>
+            <v>88.891581412358917</v>
           </cell>
         </row>
         <row r="52">
@@ -2573,16 +2573,16 @@
             <v>#N/A</v>
           </cell>
           <cell r="D52">
-            <v>53</v>
+            <v>54</v>
           </cell>
           <cell r="E52">
-            <v>56.944000000000003</v>
+            <v>55.616</v>
           </cell>
           <cell r="H52">
-            <v>34.818118559944736</v>
+            <v>34.068320116932881</v>
           </cell>
           <cell r="I52">
-            <v>93.130222714858448</v>
+            <v>90.792250553693293</v>
           </cell>
         </row>
         <row r="53">
@@ -2593,16 +2593,16 @@
             <v>#N/A</v>
           </cell>
           <cell r="D53">
-            <v>53</v>
+            <v>54</v>
           </cell>
           <cell r="E53">
-            <v>56.884</v>
-          </cell>
-          <cell r="H53" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="I53" t="e">
-            <v>#N/A</v>
+            <v>55.660000000000004</v>
+          </cell>
+          <cell r="H53">
+            <v>33.381601430531042</v>
+          </cell>
+          <cell r="I53">
+            <v>92.806679944555199</v>
           </cell>
         </row>
         <row r="54">
@@ -2613,16 +2613,16 @@
             <v>#N/A</v>
           </cell>
           <cell r="D54">
-            <v>53</v>
+            <v>54</v>
           </cell>
           <cell r="E54">
-            <v>56.823999999999998</v>
-          </cell>
-          <cell r="H54" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="I54" t="e">
-            <v>#N/A</v>
+            <v>55.694000000000003</v>
+          </cell>
+          <cell r="H54">
+            <v>32.906422271354188</v>
+          </cell>
+          <cell r="I54">
+            <v>94.261892417888561</v>
           </cell>
         </row>
         <row r="55">
@@ -2633,16 +2633,16 @@
             <v>#N/A</v>
           </cell>
           <cell r="D55">
-            <v>53</v>
+            <v>54</v>
           </cell>
           <cell r="E55">
-            <v>56.754000000000005</v>
-          </cell>
-          <cell r="H55" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="I55" t="e">
-            <v>#N/A</v>
+            <v>55.731999999999992</v>
+          </cell>
+          <cell r="H55">
+            <v>32.42676407210547</v>
+          </cell>
+          <cell r="I55">
+            <v>95.786795657230783</v>
           </cell>
         </row>
         <row r="56">
@@ -2653,16 +2653,16 @@
             <v>#N/A</v>
           </cell>
           <cell r="D56">
-            <v>54</v>
+            <v>55</v>
           </cell>
           <cell r="E56">
-            <v>56.679999999999993</v>
-          </cell>
-          <cell r="H56" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="I56" t="e">
-            <v>#N/A</v>
+            <v>55.738</v>
+          </cell>
+          <cell r="H56">
+            <v>32.033729548552806</v>
+          </cell>
+          <cell r="I56">
+            <v>96.982920433638768</v>
           </cell>
         </row>
         <row r="57">
@@ -2673,16 +2673,16 @@
             <v>#N/A</v>
           </cell>
           <cell r="D57">
-            <v>55</v>
+            <v>56</v>
           </cell>
           <cell r="E57">
-            <v>56.60799999999999</v>
-          </cell>
-          <cell r="H57" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="I57" t="e">
-            <v>#N/A</v>
+            <v>55.736000000000004</v>
+          </cell>
+          <cell r="H57">
+            <v>31.622050174373111</v>
+          </cell>
+          <cell r="I57">
+            <v>98.238465844872607</v>
           </cell>
         </row>
         <row r="58">
@@ -2693,16 +2693,16 @@
             <v>#N/A</v>
           </cell>
           <cell r="D58">
-            <v>55</v>
+            <v>56</v>
           </cell>
           <cell r="E58">
-            <v>56.564</v>
+            <v>55.725999999999999</v>
           </cell>
           <cell r="H58">
-            <v>32.021640238413859</v>
+            <v>31.421745124934933</v>
           </cell>
           <cell r="I58">
-            <v>99.916371309481718</v>
+            <v>98.82923636649636</v>
           </cell>
         </row>
         <row r="59">
@@ -2713,16 +2713,16 @@
             <v>#N/A</v>
           </cell>
           <cell r="D59">
-            <v>55</v>
+            <v>56</v>
           </cell>
           <cell r="E59">
-            <v>56.486000000000004</v>
-          </cell>
-          <cell r="H59" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="I59" t="e">
-            <v>#N/A</v>
+            <v>55.679999999999993</v>
+          </cell>
+          <cell r="H59">
+            <v>30.895951939699067</v>
+          </cell>
+          <cell r="I59">
+            <v>100.3452622547741</v>
           </cell>
         </row>
         <row r="60">
@@ -2733,16 +2733,16 @@
             <v>#N/A</v>
           </cell>
           <cell r="D60">
-            <v>56</v>
+            <v>57</v>
           </cell>
           <cell r="E60">
-            <v>56.427999999999997</v>
-          </cell>
-          <cell r="H60" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="I60" t="e">
-            <v>#N/A</v>
+            <v>55.646000000000001</v>
+          </cell>
+          <cell r="H60">
+            <v>30.59698227934512</v>
+          </cell>
+          <cell r="I60">
+            <v>101.20204952663963</v>
           </cell>
         </row>
         <row r="61">
@@ -2753,16 +2753,16 @@
             <v>#N/A</v>
           </cell>
           <cell r="D61">
-            <v>56</v>
+            <v>57</v>
           </cell>
           <cell r="E61">
-            <v>56.402000000000001</v>
-          </cell>
-          <cell r="H61" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="I61" t="e">
-            <v>#N/A</v>
+            <v>55.620000000000005</v>
+          </cell>
+          <cell r="H61">
+            <v>30.270109390498018</v>
+          </cell>
+          <cell r="I61">
+            <v>102.19931352382547</v>
           </cell>
         </row>
         <row r="62">
@@ -2773,16 +2773,16 @@
             <v>#N/A</v>
           </cell>
           <cell r="D62">
-            <v>57</v>
+            <v>58</v>
           </cell>
           <cell r="E62">
-            <v>56.386000000000003</v>
-          </cell>
-          <cell r="H62" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="I62" t="e">
-            <v>#N/A</v>
+            <v>55.608000000000004</v>
+          </cell>
+          <cell r="H62">
+            <v>30.011037641066501</v>
+          </cell>
+          <cell r="I62">
+            <v>103.03707925675414</v>
           </cell>
         </row>
         <row r="63">
@@ -2793,16 +2793,16 @@
             <v>#N/A</v>
           </cell>
           <cell r="D63">
-            <v>57</v>
+            <v>58</v>
           </cell>
           <cell r="E63">
-            <v>56.379999999999995</v>
-          </cell>
-          <cell r="H63" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="I63" t="e">
-            <v>#N/A</v>
+            <v>55.606000000000009</v>
+          </cell>
+          <cell r="H63">
+            <v>29.759663551158464</v>
+          </cell>
+          <cell r="I63">
+            <v>103.8999392813914</v>
           </cell>
         </row>
         <row r="64">
@@ -2813,16 +2813,16 @@
             <v>#N/A</v>
           </cell>
           <cell r="D64">
-            <v>58</v>
+            <v>59</v>
           </cell>
           <cell r="E64">
-            <v>56.383999999999993</v>
+            <v>55.622</v>
           </cell>
           <cell r="H64">
-            <v>30.097734612969429</v>
+            <v>29.731159362954337</v>
           </cell>
           <cell r="I64">
-            <v>105.6277323486688</v>
+            <v>104.05940939709703</v>
           </cell>
         </row>
         <row r="86">
@@ -3596,7 +3596,7 @@
         <v>42675</v>
       </c>
       <c r="C39" s="16">
-        <v>45.71</v>
+        <v>45.661000000000001</v>
       </c>
       <c r="D39" s="16" t="e">
         <v>#N/A</v>
@@ -3634,8 +3634,8 @@
       <c r="C40" s="16">
         <v>51.97</v>
       </c>
-      <c r="D40" s="16">
-        <v>51.97</v>
+      <c r="D40" s="16" t="e">
+        <v>#N/A</v>
       </c>
       <c r="E40" s="16" t="e">
         <v>#N/A</v>
@@ -3667,11 +3667,11 @@
       <c r="B41" s="12">
         <v>42736</v>
       </c>
-      <c r="C41" s="16" t="e">
-        <v>#N/A</v>
+      <c r="C41" s="16">
+        <v>52.49</v>
       </c>
       <c r="D41" s="16">
-        <v>52</v>
+        <v>52.49</v>
       </c>
       <c r="E41" s="16" t="e">
         <v>#N/A</v>
@@ -3707,7 +3707,7 @@
         <v>#N/A</v>
       </c>
       <c r="D42" s="16">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E42" s="16" t="e">
         <v>#N/A</v>
@@ -3743,32 +3743,32 @@
         <v>#N/A</v>
       </c>
       <c r="D43" s="16">
-        <v>52</v>
-      </c>
-      <c r="E43" s="16">
-        <v>54.314</v>
-      </c>
-      <c r="F43" s="17">
-        <v>0.28819824999999993</v>
-      </c>
-      <c r="G43" s="18">
-        <v>28</v>
-      </c>
-      <c r="H43" s="16">
+        <v>53</v>
+      </c>
+      <c r="E43" s="16" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F43" s="17" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G43" s="18" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H43" s="16" t="e">
         <f t="shared" si="0"/>
-        <v>44.992506655000135</v>
-      </c>
-      <c r="I43" s="16">
+        <v>#N/A</v>
+      </c>
+      <c r="I43" s="16" t="e">
         <f t="shared" si="1"/>
-        <v>65.566709110486016</v>
-      </c>
-      <c r="J43" s="2">
+        <v>#N/A</v>
+      </c>
+      <c r="J43" s="2" t="e">
         <f t="shared" si="2"/>
-        <v>44.992506653012128</v>
-      </c>
-      <c r="K43" s="2">
+        <v>#N/A</v>
+      </c>
+      <c r="K43" s="2" t="e">
         <f t="shared" si="3"/>
-        <v>65.566709113383098</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.25">
@@ -3779,32 +3779,32 @@
         <v>#N/A</v>
       </c>
       <c r="D44" s="16">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E44" s="16">
-        <v>55.116</v>
+        <v>53.814000000000007</v>
       </c>
       <c r="F44" s="17">
-        <v>0.28771150000000001</v>
+        <v>0.28439492500000002</v>
       </c>
       <c r="G44" s="18">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="H44" s="16">
         <f t="shared" si="0"/>
-        <v>43.091772909633576</v>
+        <v>44.542492128643843</v>
       </c>
       <c r="I44" s="16">
         <f t="shared" si="1"/>
-        <v>70.495439172818919</v>
+        <v>65.015369765036354</v>
       </c>
       <c r="J44" s="2">
         <f t="shared" si="2"/>
-        <v>43.091772907144836</v>
+        <v>44.542492126667327</v>
       </c>
       <c r="K44" s="2">
         <f t="shared" si="3"/>
-        <v>70.495439176890343</v>
+        <v>65.015369767921342</v>
       </c>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.25">
@@ -3815,32 +3815,32 @@
         <v>#N/A</v>
       </c>
       <c r="D45" s="16">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E45" s="16">
-        <v>55.777999999999999</v>
+        <v>54.326000000000001</v>
       </c>
       <c r="F45" s="17">
-        <v>0.28599304999999997</v>
+        <v>0.28567862499999996</v>
       </c>
       <c r="G45" s="18">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="H45" s="16">
         <f t="shared" si="0"/>
-        <v>41.598697955469788</v>
+        <v>42.334181145273284</v>
       </c>
       <c r="I45" s="16">
         <f t="shared" si="1"/>
-        <v>74.790448665735511</v>
+        <v>69.714689080020676</v>
       </c>
       <c r="J45" s="2">
         <f t="shared" si="2"/>
-        <v>41.598697952606493</v>
+        <v>42.334181142795515</v>
       </c>
       <c r="K45" s="2">
         <f t="shared" si="3"/>
-        <v>74.79044867088345</v>
+        <v>69.714689084100982</v>
       </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.25">
@@ -3851,32 +3851,32 @@
         <v>#N/A</v>
       </c>
       <c r="D46" s="16">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E46" s="16">
-        <v>56.265999999999998</v>
+        <v>54.757999999999996</v>
       </c>
       <c r="F46" s="17">
-        <v>0.28747612499999997</v>
+        <v>0.29265872500000001</v>
       </c>
       <c r="G46" s="18">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="H46" s="16">
         <f t="shared" si="0"/>
-        <v>40.105096853756812</v>
+        <v>40.298775355191346</v>
       </c>
       <c r="I46" s="16">
         <f t="shared" si="1"/>
-        <v>78.939162459682237</v>
+        <v>74.405203075575258</v>
       </c>
       <c r="J46" s="2">
         <f t="shared" si="2"/>
-        <v>40.105096850570206</v>
+        <v>40.29877535229182</v>
       </c>
       <c r="K46" s="2">
         <f t="shared" si="3"/>
-        <v>78.939162465954468</v>
+        <v>74.405203080928757</v>
       </c>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.25">
@@ -3887,32 +3887,32 @@
         <v>#N/A</v>
       </c>
       <c r="D47" s="16">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E47" s="16">
-        <v>56.573999999999998</v>
+        <v>55.064</v>
       </c>
       <c r="F47" s="17">
-        <v>0.28918141785714291</v>
+        <v>0.29874287500000002</v>
       </c>
       <c r="G47" s="18">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="H47" s="16">
         <f t="shared" si="0"/>
-        <v>38.837387675060832</v>
+        <v>38.656357360969729</v>
       </c>
       <c r="I47" s="16">
         <f t="shared" si="1"/>
-        <v>82.410730164924416</v>
+        <v>78.435846080556274</v>
       </c>
       <c r="J47" s="2">
         <f t="shared" si="2"/>
-        <v>38.837387671632456</v>
+        <v>38.656357357760363</v>
       </c>
       <c r="K47" s="2">
         <f t="shared" si="3"/>
-        <v>82.410730172199237</v>
+        <v>78.435846087068242</v>
       </c>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.25">
@@ -3923,32 +3923,32 @@
         <v>#N/A</v>
       </c>
       <c r="D48" s="16">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E48" s="16">
-        <v>56.741999999999997</v>
+        <v>55.25</v>
       </c>
       <c r="F48" s="17">
-        <v>0.28411728000000003</v>
+        <v>0.29346794761904765</v>
       </c>
       <c r="G48" s="18">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="H48" s="16">
         <f t="shared" si="0"/>
-        <v>37.920401356633704</v>
+        <v>37.588664956469671</v>
       </c>
       <c r="I48" s="16">
         <f t="shared" si="1"/>
-        <v>84.905603548860142</v>
+        <v>81.209654653472882</v>
       </c>
       <c r="J48" s="2">
         <f t="shared" si="2"/>
-        <v>37.920401353047261</v>
+        <v>37.58866495307214</v>
       </c>
       <c r="K48" s="2">
         <f t="shared" si="3"/>
-        <v>84.905603556890355</v>
+        <v>81.209654660813186</v>
       </c>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.25">
@@ -3959,32 +3959,32 @@
         <v>#N/A</v>
       </c>
       <c r="D49" s="16">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E49" s="16">
-        <v>56.844000000000008</v>
+        <v>55.379999999999995</v>
       </c>
       <c r="F49" s="17">
-        <v>0.28180594642857143</v>
+        <v>0.29255038214285711</v>
       </c>
       <c r="G49" s="18">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="H49" s="16">
         <f t="shared" si="0"/>
-        <v>36.860305349127543</v>
+        <v>36.342571643368707</v>
       </c>
       <c r="I49" s="16">
         <f t="shared" si="1"/>
-        <v>87.661789705615718</v>
+        <v>84.38985633972365</v>
       </c>
       <c r="J49" s="2">
         <f t="shared" si="2"/>
-        <v>36.86030534538056</v>
+        <v>36.342571639776246</v>
       </c>
       <c r="K49" s="2">
         <f t="shared" si="3"/>
-        <v>87.661789714526847</v>
+        <v>84.389856348065592</v>
       </c>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.25">
@@ -3995,32 +3995,32 @@
         <v>#N/A</v>
       </c>
       <c r="D50" s="16">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E50" s="16">
-        <v>56.894000000000005</v>
+        <v>55.470000000000006</v>
       </c>
       <c r="F50" s="17">
-        <v>0.27941016666666674</v>
+        <v>0.28936083333333334</v>
       </c>
       <c r="G50" s="18">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="H50" s="16">
         <f t="shared" si="0"/>
-        <v>36.04716912997808</v>
+        <v>35.503151838856461</v>
       </c>
       <c r="I50" s="16">
         <f t="shared" si="1"/>
-        <v>89.796988615898243</v>
+        <v>86.666133586271116</v>
       </c>
       <c r="J50" s="2">
         <f t="shared" si="2"/>
-        <v>36.047169126117623</v>
+        <v>35.503151835138745</v>
       </c>
       <c r="K50" s="2">
         <f t="shared" si="3"/>
-        <v>89.796988625515027</v>
+        <v>86.666133595346366</v>
       </c>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.25">
@@ -4031,32 +4031,32 @@
         <v>#N/A</v>
       </c>
       <c r="D51" s="16">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E51" s="16">
-        <v>56.922000000000004</v>
+        <v>55.548000000000002</v>
       </c>
       <c r="F51" s="17">
-        <v>0.27598726666666668</v>
+        <v>0.28623345666666672</v>
       </c>
       <c r="G51" s="18">
-        <v>196</v>
+        <v>177</v>
       </c>
       <c r="H51" s="16">
         <f t="shared" si="0"/>
-        <v>35.326408825942011</v>
+        <v>34.711726970930016</v>
       </c>
       <c r="I51" s="16">
         <f t="shared" si="1"/>
-        <v>91.719316842096248</v>
+        <v>88.891581412358917</v>
       </c>
       <c r="J51" s="2">
         <f t="shared" si="2"/>
-        <v>35.326408821987222</v>
+        <v>34.711726967100098</v>
       </c>
       <c r="K51" s="2">
         <f t="shared" si="3"/>
-        <v>91.719316852364216</v>
+        <v>88.89158142216678</v>
       </c>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.25">
@@ -4067,32 +4067,32 @@
         <v>#N/A</v>
       </c>
       <c r="D52" s="16">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E52" s="16">
-        <v>56.944000000000003</v>
+        <v>55.616</v>
       </c>
       <c r="F52" s="17">
-        <v>0.27109967142857144</v>
+        <v>0.28281760000000006</v>
       </c>
       <c r="G52" s="18">
-        <v>216</v>
+        <v>197</v>
       </c>
       <c r="H52" s="16">
         <f t="shared" si="0"/>
-        <v>34.818118559944736</v>
+        <v>34.068320116932881</v>
       </c>
       <c r="I52" s="16">
         <f t="shared" si="1"/>
-        <v>93.130222714858448</v>
+        <v>90.792250553693293</v>
       </c>
       <c r="J52" s="2">
         <f t="shared" si="2"/>
-        <v>34.818118555925274</v>
+        <v>34.068320113014586</v>
       </c>
       <c r="K52" s="2">
         <f t="shared" si="3"/>
-        <v>93.130222725609556</v>
+        <v>90.792250564135585</v>
       </c>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.25">
@@ -4103,32 +4103,32 @@
         <v>#N/A</v>
       </c>
       <c r="D53" s="16">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E53" s="16">
-        <v>56.884</v>
-      </c>
-      <c r="F53" s="17" t="e">
-        <v>#N/A</v>
+        <v>55.660000000000004</v>
+      </c>
+      <c r="F53" s="17">
+        <v>0.28110040000000003</v>
       </c>
       <c r="G53" s="18">
-        <v>236</v>
-      </c>
-      <c r="H53" s="16" t="e">
+        <v>217</v>
+      </c>
+      <c r="H53" s="16">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I53" s="16" t="e">
+        <v>33.381601430531042</v>
+      </c>
+      <c r="I53" s="16">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="J53" s="2" t="e">
+        <v>92.806679944555199</v>
+      </c>
+      <c r="J53" s="2">
         <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="K53" s="2" t="e">
+        <v>33.381601426526018</v>
+      </c>
+      <c r="K53" s="2">
         <f t="shared" si="3"/>
-        <v>#N/A</v>
+        <v>92.806679955689859</v>
       </c>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.25">
@@ -4139,32 +4139,32 @@
         <v>#N/A</v>
       </c>
       <c r="D54" s="16">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E54" s="16">
-        <v>56.823999999999998</v>
-      </c>
-      <c r="F54" s="17" t="e">
-        <v>#N/A</v>
+        <v>55.694000000000003</v>
+      </c>
+      <c r="F54" s="17">
+        <v>0.27626020000000001</v>
       </c>
       <c r="G54" s="18">
-        <v>257</v>
-      </c>
-      <c r="H54" s="16" t="e">
+        <v>238</v>
+      </c>
+      <c r="H54" s="16">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I54" s="16" t="e">
+        <v>32.906422271354188</v>
+      </c>
+      <c r="I54" s="16">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="J54" s="2" t="e">
+        <v>94.261892417888561</v>
+      </c>
+      <c r="J54" s="2">
         <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="K54" s="2" t="e">
+        <v>32.906422267290743</v>
+      </c>
+      <c r="K54" s="2">
         <f t="shared" si="3"/>
-        <v>#N/A</v>
+        <v>94.261892429528487</v>
       </c>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.25">
@@ -4175,32 +4175,32 @@
         <v>#N/A</v>
       </c>
       <c r="D55" s="16">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E55" s="16">
-        <v>56.754000000000005</v>
-      </c>
-      <c r="F55" s="17" t="e">
-        <v>#N/A</v>
+        <v>55.731999999999992</v>
+      </c>
+      <c r="F55" s="17">
+        <v>0.27308459999999996</v>
       </c>
       <c r="G55" s="18">
-        <v>277</v>
-      </c>
-      <c r="H55" s="16" t="e">
+        <v>258</v>
+      </c>
+      <c r="H55" s="16">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I55" s="16" t="e">
+        <v>32.42676407210547</v>
+      </c>
+      <c r="I55" s="16">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="J55" s="2" t="e">
+        <v>95.786795657230783</v>
+      </c>
+      <c r="J55" s="2">
         <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="K55" s="2" t="e">
+        <v>32.426764067984337</v>
+      </c>
+      <c r="K55" s="2">
         <f t="shared" si="3"/>
-        <v>#N/A</v>
+        <v>95.78679566940437</v>
       </c>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.25">
@@ -4211,32 +4211,32 @@
         <v>#N/A</v>
       </c>
       <c r="D56" s="16">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E56" s="16">
-        <v>56.679999999999993</v>
-      </c>
-      <c r="F56" s="17" t="e">
-        <v>#N/A</v>
+        <v>55.738</v>
+      </c>
+      <c r="F56" s="17">
+        <v>0.26905420000000002</v>
       </c>
       <c r="G56" s="18">
-        <v>297</v>
-      </c>
-      <c r="H56" s="16" t="e">
+        <v>278</v>
+      </c>
+      <c r="H56" s="16">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I56" s="16" t="e">
+        <v>32.033729548552806</v>
+      </c>
+      <c r="I56" s="16">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="J56" s="2" t="e">
+        <v>96.982920433638768</v>
+      </c>
+      <c r="J56" s="2">
         <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="K56" s="2" t="e">
+        <v>32.033729544389139</v>
+      </c>
+      <c r="K56" s="2">
         <f t="shared" si="3"/>
-        <v>#N/A</v>
+        <v>96.982920446244378</v>
       </c>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.25">
@@ -4247,32 +4247,32 @@
         <v>#N/A</v>
       </c>
       <c r="D57" s="16">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E57" s="16">
-        <v>56.60799999999999</v>
-      </c>
-      <c r="F57" s="17" t="e">
-        <v>#N/A</v>
+        <v>55.736000000000004</v>
+      </c>
+      <c r="F57" s="17">
+        <v>0.26503280000000001</v>
       </c>
       <c r="G57" s="18">
-        <v>319</v>
-      </c>
-      <c r="H57" s="16" t="e">
+        <v>300</v>
+      </c>
+      <c r="H57" s="16">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I57" s="16" t="e">
+        <v>31.622050174373111</v>
+      </c>
+      <c r="I57" s="16">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="J57" s="2" t="e">
+        <v>98.238465844872607</v>
+      </c>
+      <c r="J57" s="2">
         <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="K57" s="2" t="e">
+        <v>31.622050170167231</v>
+      </c>
+      <c r="K57" s="2">
         <f t="shared" si="3"/>
-        <v>#N/A</v>
+        <v>98.238465857938778</v>
       </c>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.25">
@@ -4283,32 +4283,32 @@
         <v>#N/A</v>
       </c>
       <c r="D58" s="16">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E58" s="16">
-        <v>56.564</v>
+        <v>55.725999999999999</v>
       </c>
       <c r="F58" s="17">
-        <v>0.24954986666666668</v>
+        <v>0.2586059</v>
       </c>
       <c r="G58" s="18">
-        <v>341</v>
+        <v>322</v>
       </c>
       <c r="H58" s="16">
         <f t="shared" si="0"/>
-        <v>32.021640238413859</v>
+        <v>31.421745124934933</v>
       </c>
       <c r="I58" s="16">
         <f t="shared" si="1"/>
-        <v>99.916371309481718</v>
+        <v>98.82923636649636</v>
       </c>
       <c r="J58" s="2">
         <f t="shared" si="2"/>
-        <v>32.021640234138381</v>
+        <v>31.421745120710167</v>
       </c>
       <c r="K58" s="2">
         <f t="shared" si="3"/>
-        <v>99.9163713228224</v>
+        <v>98.829236379784334</v>
       </c>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.25">
@@ -4319,32 +4319,32 @@
         <v>#N/A</v>
       </c>
       <c r="D59" s="16">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E59" s="16">
-        <v>56.486000000000004</v>
-      </c>
-      <c r="F59" s="17" t="e">
-        <v>#N/A</v>
+        <v>55.679999999999993</v>
+      </c>
+      <c r="F59" s="17">
+        <v>0.25795940000000001</v>
       </c>
       <c r="G59" s="18">
-        <v>361</v>
-      </c>
-      <c r="H59" s="16" t="e">
+        <v>342</v>
+      </c>
+      <c r="H59" s="16">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I59" s="16" t="e">
+        <v>30.895951939699067</v>
+      </c>
+      <c r="I59" s="16">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="J59" s="2" t="e">
+        <v>100.3452622547741</v>
+      </c>
+      <c r="J59" s="2">
         <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="K59" s="2" t="e">
+        <v>30.895951935428624</v>
+      </c>
+      <c r="K59" s="2">
         <f t="shared" si="3"/>
-        <v>#N/A</v>
+        <v>100.34526226864382</v>
       </c>
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.25">
@@ -4355,32 +4355,32 @@
         <v>#N/A</v>
       </c>
       <c r="D60" s="16">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E60" s="16">
-        <v>56.427999999999997</v>
-      </c>
-      <c r="F60" s="17" t="e">
-        <v>#N/A</v>
+        <v>55.646000000000001</v>
+      </c>
+      <c r="F60" s="17">
+        <v>0.2542606</v>
       </c>
       <c r="G60" s="18">
-        <v>382</v>
-      </c>
-      <c r="H60" s="16" t="e">
+        <v>363</v>
+      </c>
+      <c r="H60" s="16">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I60" s="16" t="e">
+        <v>30.59698227934512</v>
+      </c>
+      <c r="I60" s="16">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="J60" s="2" t="e">
+        <v>101.20204952663963</v>
+      </c>
+      <c r="J60" s="2">
         <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="K60" s="2" t="e">
+        <v>30.596982275050568</v>
+      </c>
+      <c r="K60" s="2">
         <f t="shared" si="3"/>
-        <v>#N/A</v>
+        <v>101.2020495408442</v>
       </c>
     </row>
     <row r="61" spans="2:11" x14ac:dyDescent="0.25">
@@ -4391,32 +4391,32 @@
         <v>#N/A</v>
       </c>
       <c r="D61" s="16">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E61" s="16">
-        <v>56.402000000000001</v>
-      </c>
-      <c r="F61" s="17" t="e">
-        <v>#N/A</v>
+        <v>55.620000000000005</v>
+      </c>
+      <c r="F61" s="17">
+        <v>0.25112980000000001</v>
       </c>
       <c r="G61" s="18">
-        <v>404</v>
-      </c>
-      <c r="H61" s="16" t="e">
+        <v>385</v>
+      </c>
+      <c r="H61" s="16">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I61" s="16" t="e">
+        <v>30.270109390498018</v>
+      </c>
+      <c r="I61" s="16">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="J61" s="2" t="e">
+        <v>102.19931352382547</v>
+      </c>
+      <c r="J61" s="2">
         <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="K61" s="2" t="e">
+        <v>30.270109386176372</v>
+      </c>
+      <c r="K61" s="2">
         <f t="shared" si="3"/>
-        <v>#N/A</v>
+        <v>102.19931353841642</v>
       </c>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.25">
@@ -4427,32 +4427,32 @@
         <v>#N/A</v>
       </c>
       <c r="D62" s="16">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E62" s="16">
-        <v>56.386000000000003</v>
-      </c>
-      <c r="F62" s="17" t="e">
-        <v>#N/A</v>
+        <v>55.608000000000004</v>
+      </c>
+      <c r="F62" s="17">
+        <v>0.24791719999999998</v>
       </c>
       <c r="G62" s="18">
-        <v>425</v>
-      </c>
-      <c r="H62" s="16" t="e">
+        <v>406</v>
+      </c>
+      <c r="H62" s="16">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I62" s="16" t="e">
+        <v>30.011037641066501</v>
+      </c>
+      <c r="I62" s="16">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="J62" s="2" t="e">
+        <v>103.03707925675414</v>
+      </c>
+      <c r="J62" s="2">
         <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="K62" s="2" t="e">
+        <v>30.011037636722818</v>
+      </c>
+      <c r="K62" s="2">
         <f t="shared" si="3"/>
-        <v>#N/A</v>
+        <v>103.03707927166731</v>
       </c>
     </row>
     <row r="63" spans="2:11" x14ac:dyDescent="0.25">
@@ -4463,32 +4463,32 @@
         <v>#N/A</v>
       </c>
       <c r="D63" s="16">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E63" s="16">
-        <v>56.379999999999995</v>
-      </c>
-      <c r="F63" s="17" t="e">
-        <v>#N/A</v>
+        <v>55.606000000000009</v>
+      </c>
+      <c r="F63" s="17">
+        <v>0.24502679999999999</v>
       </c>
       <c r="G63" s="18">
-        <v>446</v>
-      </c>
-      <c r="H63" s="16" t="e">
+        <v>427</v>
+      </c>
+      <c r="H63" s="16">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I63" s="16" t="e">
+        <v>29.759663551158464</v>
+      </c>
+      <c r="I63" s="16">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="J63" s="2" t="e">
+        <v>103.8999392813914</v>
+      </c>
+      <c r="J63" s="2">
         <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="K63" s="2" t="e">
+        <v>29.75966354679268</v>
+      </c>
+      <c r="K63" s="2">
         <f t="shared" si="3"/>
-        <v>#N/A</v>
+        <v>103.89993929663366</v>
       </c>
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.25">
@@ -4499,32 +4499,32 @@
         <v>#N/A</v>
       </c>
       <c r="D64" s="20">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E64" s="20">
-        <v>56.383999999999993</v>
+        <v>55.622</v>
       </c>
       <c r="F64" s="21">
-        <v>0.23577752738095242</v>
+        <v>0.24022866785714286</v>
       </c>
       <c r="G64" s="22">
-        <v>465</v>
+        <v>446</v>
       </c>
       <c r="H64" s="20">
         <f t="shared" si="0"/>
-        <v>30.097734612969429</v>
+        <v>29.731159362954337</v>
       </c>
       <c r="I64" s="20">
         <f t="shared" si="1"/>
-        <v>105.6277323486688</v>
+        <v>104.05940939709703</v>
       </c>
       <c r="J64" s="2">
         <f t="shared" si="2"/>
-        <v>30.097734608535696</v>
+        <v>29.731159358584041</v>
       </c>
       <c r="K64" s="2">
         <f t="shared" si="3"/>
-        <v>105.62773236422893</v>
+        <v>104.05940941239312</v>
       </c>
     </row>
     <row r="65" spans="2:13" x14ac:dyDescent="0.25">

</xml_diff>